<commit_message>
buncha updates - catch up from weekend
</commit_message>
<xml_diff>
--- a/EC/Train Runs and Enforcements 2016-07-27.xlsx
+++ b/EC/Train Runs and Enforcements 2016-07-27.xlsx
@@ -3114,37 +3114,7 @@
     <cellStyle name="Normal_XINGS" xfId="1"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -3508,8 +3478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CM214"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X19" sqref="X19:X29"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="L48" sqref="L48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26858,27 +26828,27 @@
     <mergeCell ref="A11:P11"/>
   </mergeCells>
   <conditionalFormatting sqref="W11:W12 W13:X1048576">
-    <cfRule type="cellIs" dxfId="11" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="76" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X13:X1048576">
-    <cfRule type="cellIs" dxfId="10" priority="59" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="59" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X12:X1048576">
-    <cfRule type="cellIs" dxfId="9" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="56" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K210:S214 K209:M209 A123:M208 N123:S209 A13:S122">
-    <cfRule type="expression" dxfId="8" priority="52">
+    <cfRule type="expression" dxfId="5" priority="52">
       <formula>$O13&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K210:S214 K209:M209 A123:M208 N123:S209 A13:S122">
-    <cfRule type="expression" dxfId="7" priority="51">
+    <cfRule type="expression" dxfId="4" priority="51">
       <formula>$P13&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -32537,17 +32507,17 @@
     <mergeCell ref="A5:M5"/>
   </mergeCells>
   <conditionalFormatting sqref="M6:N6 P6 M7:M1048576">
-    <cfRule type="cellIs" dxfId="5" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="14" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:N66">
-    <cfRule type="expression" dxfId="4" priority="7">
+    <cfRule type="expression" dxfId="1" priority="7">
       <formula>$M7="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M3">
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
update desc for 122
</commit_message>
<xml_diff>
--- a/EC/Train Runs and Enforcements 2016-07-27.xlsx
+++ b/EC/Train Runs and Enforcements 2016-07-27.xlsx
@@ -2428,9 +2428,6 @@
     <t>DUS 2N was STOP, no clear request sent until after train was cut out (inefficient dispatching)</t>
   </si>
   <si>
-    <t>Sand Creek 4S was STOP, track circuit/occupation issue</t>
-  </si>
-  <si>
     <t>Form C</t>
   </si>
   <si>
@@ -2474,6 +2471,9 @@
   </si>
   <si>
     <t>No initialization attempt recorded</t>
+  </si>
+  <si>
+    <t>Sand Creek 4S was STOP, signal system performed as designed. Interaction with Ulster and train behind</t>
   </si>
 </sst>
 </file>
@@ -3478,8 +3478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CM214"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="L48" sqref="L48"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="R34" sqref="R34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5193,7 +5193,7 @@
         <v>727</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="C22" s="25" t="s">
         <v>184</v>
@@ -5205,7 +5205,7 @@
         <v>42578.197094907409</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="G22" s="7">
         <v>1</v>
@@ -5214,7 +5214,7 @@
         <v>179</v>
       </c>
       <c r="I22" s="16" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="J22" s="7">
         <v>0</v>
@@ -5238,7 +5238,7 @@
       </c>
       <c r="Q22" s="26"/>
       <c r="R22" s="26" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="S22" s="41">
         <f t="shared" ref="S22" si="22">SUM(U22:U22)/IF(AG22="EC",12,1)</f>
@@ -5531,28 +5531,28 @@
         <v>728</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="D25" s="25" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="E25" s="16" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="F25" s="16" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="H25" s="16" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="I25" s="16" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="J25" s="7">
         <v>0</v>
@@ -5576,7 +5576,7 @@
       </c>
       <c r="Q25" s="26"/>
       <c r="R25" s="26" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="S25" s="41">
         <f t="shared" ref="S25:S26" si="35">SUM(U25:U25)/IF(AG25="EC",12,1)</f>
@@ -5645,28 +5645,28 @@
         <v>729</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="F26" s="16" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="H26" s="16" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="I26" s="16" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="J26" s="7">
         <v>0</v>
@@ -5690,7 +5690,7 @@
       </c>
       <c r="Q26" s="26"/>
       <c r="R26" s="26" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="S26" s="41">
         <f t="shared" si="35"/>
@@ -6588,7 +6588,7 @@
       </c>
       <c r="Q34" s="26"/>
       <c r="R34" s="26" t="s">
-        <v>788</v>
+        <v>803</v>
       </c>
       <c r="S34" s="41">
         <f>SUM(U34:U35)/IF(AG34="EC",12,1)</f>
@@ -26943,7 +26943,7 @@
         <v>4038</v>
       </c>
       <c r="D3" s="37" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="E3" s="25" t="e">
         <f>VLOOKUP(A3,'Trips&amp;Operators'!$C$2:$E$10000,3,FALSE)</f>
@@ -26975,7 +26975,7 @@
         <v>730</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="E4" s="25" t="e">
         <f>VLOOKUP(A4,'Trips&amp;Operators'!$C$2:$E$10000,3,FALSE)</f>
@@ -27007,7 +27007,7 @@
         <v>4009</v>
       </c>
       <c r="D5" s="37" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="E5" s="25" t="e">
         <f>VLOOKUP(A5,'Trips&amp;Operators'!$C$2:$E$10000,3,FALSE)</f>
@@ -27039,7 +27039,7 @@
         <v>783</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="E6" s="25" t="e">
         <f>VLOOKUP(A6,'Trips&amp;Operators'!$C$2:$E$10000,3,FALSE)</f>
@@ -27071,7 +27071,7 @@
         <v>783</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="E7" s="25" t="e">
         <f>VLOOKUP(A7,'Trips&amp;Operators'!$C$2:$E$10000,3,FALSE)</f>
@@ -27103,7 +27103,7 @@
         <v>0</v>
       </c>
       <c r="D8" s="37" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E8" s="25" t="e">
         <f>VLOOKUP(A8,'Trips&amp;Operators'!$C$2:$E$10000,3,FALSE)</f>
@@ -28618,7 +28618,7 @@
         <v>97</v>
       </c>
       <c r="N13" s="10" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="O13" s="37"/>
       <c r="P13" s="63" t="str">
@@ -28692,7 +28692,7 @@
         <v>97</v>
       </c>
       <c r="N14" s="10" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="O14" s="37"/>
       <c r="P14" s="63" t="str">
@@ -28766,7 +28766,7 @@
         <v>97</v>
       </c>
       <c r="N15" s="10" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="O15" s="37"/>
       <c r="P15" s="63" t="str">
@@ -29638,7 +29638,7 @@
         <v>97</v>
       </c>
       <c r="N27" s="10" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="O27" s="37"/>
       <c r="P27" s="63" t="str">
@@ -29712,7 +29712,7 @@
         <v>97</v>
       </c>
       <c r="N28" s="10" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="O28" s="37"/>
       <c r="P28" s="63" t="str">
@@ -29786,7 +29786,7 @@
         <v>96</v>
       </c>
       <c r="N29" s="10" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="O29" s="37"/>
       <c r="P29" s="63" t="str">
@@ -29860,7 +29860,7 @@
         <v>97</v>
       </c>
       <c r="N30" s="10" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="O30" s="37"/>
       <c r="P30" s="63" t="str">
@@ -29934,7 +29934,7 @@
         <v>97</v>
       </c>
       <c r="N31" s="10" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="O31" s="37"/>
       <c r="P31" s="63" t="str">
@@ -30008,7 +30008,7 @@
         <v>97</v>
       </c>
       <c r="N32" s="10" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="O32" s="37"/>
       <c r="P32" s="63" t="str">
@@ -30082,7 +30082,7 @@
         <v>97</v>
       </c>
       <c r="N33" s="10" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="O33" s="37"/>
       <c r="P33" s="63" t="str">
@@ -30156,7 +30156,7 @@
         <v>96</v>
       </c>
       <c r="N34" s="10" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="O34" s="37"/>
       <c r="P34" s="63" t="str">
@@ -31526,7 +31526,7 @@
         <v>96</v>
       </c>
       <c r="N53" s="10" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="O53" s="37"/>
       <c r="P53" s="63" t="str">

</xml_diff>